<commit_message>
project adds a barchart to spreadsheet
</commit_message>
<xml_diff>
--- a/PythonBasics/exelAutomationProject/transactions2.xlsx
+++ b/PythonBasics/exelAutomationProject/transactions2.xlsx
@@ -162,6 +162,90 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -446,7 +530,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -533,5 +617,6 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>